<commit_message>
updated ml & ts
</commit_message>
<xml_diff>
--- a/data/sample data/pres_sample.xlsx
+++ b/data/sample data/pres_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlin/PycharmProjects/thesis/data/sample data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlin/Desktop/honors-thesis/data/sample data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EF9F40-2F6B-3245-B3A7-E932F0E57427}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1870D325-8CBE-814C-B546-CAAB1AC35264}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1400" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3451,7 +3451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3461,6 +3461,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3494,7 +3502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3507,6 +3515,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3849,8 +3860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B147" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6022,7 +6033,7 @@
       <c r="D98" t="s">
         <v>488</v>
       </c>
-      <c r="E98" s="4" t="s">
+      <c r="E98" s="6" t="s">
         <v>486</v>
       </c>
       <c r="F98" t="s">

</xml_diff>